<commit_message>
Prva skica baze sa početnim punjenjem (liquibase deployment)
Testirano sa postgres:latest sa docker hub. Očekuje da je baza ni već kreirana na serveru.
</commit_message>
<xml_diff>
--- a/Dokumenti/Sifarnici.xlsx
+++ b/Dokumenti/Sifarnici.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\einicijative\Dokumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05737BF-3A8F-47EB-B118-69D00A9D6E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CABA51-3BE7-4CED-B495-A565A04C04C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TipKorisnika" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="510">
   <si>
     <t>70092</t>
   </si>
@@ -1260,9 +1260,6 @@
     <t>БРН</t>
   </si>
   <si>
-    <t>ШУМ</t>
-  </si>
-  <si>
     <t>БРС</t>
   </si>
   <si>
@@ -1309,9 +1306,6 @@
   </si>
   <si>
     <t>КПМ</t>
-  </si>
-  <si>
-    <t>V</t>
   </si>
   <si>
     <t>ШМД</t>
@@ -2028,6 +2022,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C69DB36-9E71-4E13-BA83-5A5D57CCF663}">
   <dimension ref="A1:D3"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="83.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>507</v>
+      </c>
+      <c r="C2" t="s">
+        <v>508</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xlfn.CONCAT("insert into NITipKorisnika(IDNITipKorisnika, Opis, Sortiranje) values ('",B2,"','",C2,"',",A2,");")</f>
+        <v>insert into NITipKorisnika(IDNITipKorisnika, Opis, Sortiranje) values ('Г','Грађанин',1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>469</v>
+      </c>
+      <c r="C3" t="s">
+        <v>509</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.CONCAT("insert into NITipKorisnika(IDNITipKorisnika, Opis, Sortiranje) values ('",B3,"','",C3,"',",A3,");")</f>
+        <v>insert into NITipKorisnika(IDNITipKorisnika, Opis, Sortiranje) values ('О','Овлашћено лице',2);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D71AAA-9F5E-4550-8FBA-49D957296867}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2040,16 +2098,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>429</v>
-      </c>
       <c r="D1" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2057,14 +2115,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>509</v>
+        <v>463</v>
       </c>
       <c r="C2" t="s">
-        <v>510</v>
+        <v>464</v>
       </c>
       <c r="D2" t="str">
-        <f>_xlfn.CONCAT("insert into NITipKorisnika(IDNITipKorisnika, Opis, Sortiranje) values ('",B2,"','",C2,"',",A2,");")</f>
-        <v>insert into NITipKorisnika(IDNITipKorisnika, Opis, Sortiranje) values ('Г','Грађанин',1);</v>
+        <f>_xlfn.CONCAT("insert into NIPol(IDNIPol, Opis, Sortiranje) values ('",B2,"','",C2,"',",A2,");")</f>
+        <v>insert into NIPol(IDNIPol, Opis, Sortiranje) values ('М','Мушки',1);</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2073,74 +2131,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="C3" t="s">
-        <v>511</v>
-      </c>
-      <c r="D3" t="str">
-        <f>_xlfn.CONCAT("insert into NITipKorisnika(IDNITipKorisnika, Opis, Sortiranje) values ('",B3,"','",C3,"',",A3,");")</f>
-        <v>insert into NITipKorisnika(IDNITipKorisnika, Opis, Sortiranje) values ('О','Овлашћено лице',2);</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D71AAA-9F5E-4550-8FBA-49D957296867}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>427</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>429</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>465</v>
-      </c>
-      <c r="C2" t="s">
         <v>466</v>
-      </c>
-      <c r="D2" t="str">
-        <f>_xlfn.CONCAT("insert into NIPol(IDNIPol, Opis, Sortiranje) values ('",B2,"','",C2,"',",A2,");")</f>
-        <v>insert into NIPol(IDNIPol, Opis, Sortiranje) values ('М','Мушки',1);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>467</v>
-      </c>
-      <c r="C3" t="s">
-        <v>468</v>
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT("insert into NIPol(IDNIPol, Opis, Sortiranje) values ('",B3,"','",C3,"',",A3,");")</f>
@@ -2171,19 +2165,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>429</v>
-      </c>
       <c r="D1" s="9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2191,10 +2185,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT("    {""idNivoaVlasti"": """,B2,""",""opis"": """,C2,""",""sortiranje"": ",A2,"},")</f>
@@ -2211,10 +2205,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT("    {""idNivoaVlasti"": """,B3,""",""opis"": """,C3,""",""sortiranje"": ",A3,"},")</f>
@@ -2231,10 +2225,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT("    {""idNivoaVlasti"": """,B4,""",""opis"": """,C4,""",""sortiranje"": ",A4,"},")</f>
@@ -2269,19 +2263,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>429</v>
-      </c>
       <c r="D1" s="9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2289,10 +2283,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT("    {""idTipaInicijative"": """,B2,""",""opis"": """,C2,""",""sortiranje"": ",A2,"},")</f>
@@ -2309,10 +2303,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D4" si="0">_xlfn.CONCAT("    {""idTipaInicijative"": """,B3,""",""opis"": """,C3,""",""sortiranje"": ",A3,"},")</f>
@@ -2329,10 +2323,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -2349,10 +2343,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D9" si="3">_xlfn.CONCAT("    {""idTipaInicijative"": """,B5,""",""opis"": """,C5,""",""sortiranje"": ",A5,"},")</f>
@@ -2369,10 +2363,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C6" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="3"/>
@@ -2389,10 +2383,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C7" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="3"/>
@@ -2409,10 +2403,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="3"/>
@@ -2429,10 +2423,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C9" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="3"/>
@@ -2452,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3227336-4F9C-4797-B505-295A045F63C3}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2468,22 +2462,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>429</v>
-      </c>
       <c r="D1" s="9" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2491,21 +2485,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E2" t="str">
         <f>_xlfn.CONCAT("    {""idFazeObrade"": """,B2,""",""opis"": """,C2,""",""sortiranje"": ",A2,",""dozvoljeneSledeceFaze"":""",D2,"""},")</f>
         <v xml:space="preserve">    {"idFazeObrade": "У","opis": "У припреми","sortiranje": 1,"dozvoljeneSledeceFaze":"В"},</v>
       </c>
       <c r="F2" t="str">
-        <f>_xlfn.CONCAT("insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('",B2,"','",C2,"',",A2,",",IF(ISBLANK(D2),"null",_xlfn.CONCAT("'",D2,"'")),");")</f>
-        <v>insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('У','У припреми',1,'В');</v>
+        <f>_xlfn.CONCAT("insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('",B2,"','",C2,"',",A2,",",IF(ISBLANK(D2),"null",_xlfn.CONCAT("'",D2,"'")),");")</f>
+        <v>insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('У','У припреми',1,'В');</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2514,21 +2508,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E9" si="0">_xlfn.CONCAT("    {""idFazeObrade"": """,B3,""",""opis"": """,C3,""",""sortiranje"": ",A3,",""dozvoljeneSledeceFaze"":""",D3,"""},")</f>
         <v xml:space="preserve">    {"idFazeObrade": "В","opis": "Поднета на верификацију скупштини","sortiranje": 2,"dozvoljeneSledeceFaze":"АБ"},</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F9" si="1">_xlfn.CONCAT("insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('",B3,"','",C3,"',",A3,",",IF(ISBLANK(D3),"null",_xlfn.CONCAT("'",D3,"'")),");")</f>
-        <v>insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('В','Поднета на верификацију скупштини',2,'АБ');</v>
+        <f t="shared" ref="F3:F9" si="1">_xlfn.CONCAT("insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('",B3,"','",C3,"',",A3,",",IF(ISBLANK(D3),"null",_xlfn.CONCAT("'",D3,"'")),");")</f>
+        <v>insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('В','Поднета на верификацију скупштини',2,'АБ');</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2537,13 +2531,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -2551,7 +2545,7 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('А','Активна (прикупљање потписа у току)',3,'ПНО');</v>
+        <v>insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('А','Активна (прикупљање потписа у току)',3,'ПНО');</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2560,13 +2554,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -2574,7 +2568,7 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('П','Покренута (скупљено довољно потписа)',4,'К');</v>
+        <v>insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('П','Покренута (скупљено довољно потписа)',4,'К');</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2583,10 +2577,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E6" t="str">
         <f>_xlfn.CONCAT("    {""idFazeObrade"": """,B6,""",""opis"": """,C6,""",""sortiranje"": ",A6,",""dozvoljeneSledeceFaze"":""",D6,"""},")</f>
@@ -2594,7 +2588,7 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('К','Комплетирана (скупштина одлучивала)',5,null);</v>
+        <v>insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('К','Комплетирана (скупштина одлучивала)',5,null);</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2603,10 +2597,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -2614,7 +2608,7 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('Н','Неуспешна (није скупљено довољно потписа)',6,null);</v>
+        <v>insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('Н','Неуспешна (није скупљено довољно потписа)',6,null);</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2623,10 +2617,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -2634,7 +2628,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('Б','Одбијена на верификацији',7,null);</v>
+        <v>insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('Б','Одбијена на верификацији',7,null);</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2643,10 +2637,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C9" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -2654,7 +2648,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIFazaObrade(IDNNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('О','Повучена (иницијативни одбор одустао)',8,null);</v>
+        <v>insert into NIFazaObrade(IDNIFazaObrade, Opis, Sortiranje, DozvoljeneSledeceFaze) values ('О','Повучена (иницијативни одбор одустао)',8,null);</v>
       </c>
     </row>
   </sheetData>
@@ -2666,7 +2660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4783239-902E-44FC-9E7D-26A4F12975F0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2678,16 +2674,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>429</v>
-      </c>
       <c r="D1" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2695,10 +2691,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT("insert into NIPokrajina(IDNIPokrajina, Opis, Sortiranje) values ('",B2,"','",C2,"',",A2,");")</f>
@@ -2726,19 +2722,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>429</v>
-      </c>
       <c r="D1" s="9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2749,7 +2745,7 @@
         <v>394</v>
       </c>
       <c r="C2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT("    {""idUpravnogOkruga"": """,B2,""",""opis"": """,C2,""",""sortiranje"": ",A2,"},")</f>
@@ -2769,7 +2765,7 @@
         <v>395</v>
       </c>
       <c r="C3" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT("    {""idUpravnogOkruga"": """,B3,""",""opis"": """,C3,""",""sortiranje"": ",A3,"},")</f>
@@ -2789,7 +2785,7 @@
         <v>396</v>
       </c>
       <c r="C4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:D31" si="1">_xlfn.CONCAT("    {""idUpravnogOkruga"": """,B4,""",""opis"": """,C4,""",""sortiranje"": ",A4,"},")</f>
@@ -2809,7 +2805,7 @@
         <v>397</v>
       </c>
       <c r="C5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
@@ -2829,7 +2825,7 @@
         <v>398</v>
       </c>
       <c r="C6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
@@ -2849,7 +2845,7 @@
         <v>399</v>
       </c>
       <c r="C7" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
@@ -2869,7 +2865,7 @@
         <v>400</v>
       </c>
       <c r="C8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
@@ -2889,7 +2885,7 @@
         <v>401</v>
       </c>
       <c r="C9" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
@@ -2909,7 +2905,7 @@
         <v>402</v>
       </c>
       <c r="C10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="1"/>
@@ -2929,7 +2925,7 @@
         <v>403</v>
       </c>
       <c r="C11" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
@@ -2949,7 +2945,7 @@
         <v>404</v>
       </c>
       <c r="C12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="1"/>
@@ -2969,7 +2965,7 @@
         <v>405</v>
       </c>
       <c r="C13" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
@@ -2986,10 +2982,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
@@ -3006,10 +3002,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C15" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
@@ -3026,10 +3022,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
@@ -3046,10 +3042,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C17" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
@@ -3066,10 +3062,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C18" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
@@ -3086,10 +3082,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C19" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
@@ -3106,10 +3102,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C20" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
@@ -3126,10 +3122,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C21" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
@@ -3146,10 +3142,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C22" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
@@ -3166,10 +3162,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C23" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
@@ -3186,10 +3182,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C24" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
@@ -3206,10 +3202,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C25" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
@@ -3226,10 +3222,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C26" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
@@ -3246,10 +3242,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C27" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
@@ -3266,10 +3262,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C28" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="1"/>
@@ -3286,10 +3282,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C29" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="1"/>
@@ -3306,10 +3302,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C30" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
@@ -3326,10 +3322,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C31" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="1"/>
@@ -3366,28 +3362,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>431</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -3862,19 +3858,19 @@
       <c r="D19" t="s">
         <v>395</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>423</v>
+      <c r="E19" t="s">
+        <v>491</v>
       </c>
       <c r="F19">
         <v>27612</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80071","opis": "Бачка Топола","sortiranje": 18,"brojRegistrovanihGlasaca":27612,"idUpravnogOkruga":"СБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80071","opis": "Бачка Топола","sortiranje": 18,"brojRegistrovanihGlasaca":27612,"idUpravnogOkruga":"СБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80071','Бачка Топола',18,27612,'СБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80071','Бачка Топола',18,27612,'СБЧ','В');</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -3891,19 +3887,19 @@
       <c r="D20" t="s">
         <v>395</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>423</v>
+      <c r="E20" t="s">
+        <v>491</v>
       </c>
       <c r="F20">
         <v>10001</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80241","opis": "Мали Иђош","sortiranje": 19,"brojRegistrovanihGlasaca":10001,"idUpravnogOkruga":"СБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80241","opis": "Мали Иђош","sortiranje": 19,"brojRegistrovanihGlasaca":10001,"idUpravnogOkruga":"СБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80241','Мали Иђош',19,10001,'СБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80241','Мали Иђош',19,10001,'СБЧ','В');</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -3920,19 +3916,19 @@
       <c r="D21" t="s">
         <v>395</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>423</v>
+      <c r="E21" t="s">
+        <v>491</v>
       </c>
       <c r="F21">
         <v>125986</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80438","opis": "Суботица","sortiranje": 20,"brojRegistrovanihGlasaca":125986,"idUpravnogOkruga":"СБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80438","opis": "Суботица","sortiranje": 20,"brojRegistrovanihGlasaca":125986,"idUpravnogOkruga":"СБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80438','Суботица',20,125986,'СБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80438','Суботица',20,125986,'СБЧ','В');</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -3949,19 +3945,19 @@
       <c r="D22" t="s">
         <v>396</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>423</v>
+      <c r="E22" t="s">
+        <v>491</v>
       </c>
       <c r="F22">
         <v>13670</v>
       </c>
       <c r="G22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80144","opis": "Житиште","sortiranje": 21,"brojRegistrovanihGlasaca":13670,"idUpravnogOkruga":"СРБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80144","opis": "Житиште","sortiranje": 21,"brojRegistrovanihGlasaca":13670,"idUpravnogOkruga":"СРБ","idPokrajine":"В"},</v>
       </c>
       <c r="H22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80144','Житиште',21,13670,'СРБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80144','Житиште',21,13670,'СРБ','В');</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -3978,19 +3974,19 @@
       <c r="D23" t="s">
         <v>396</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>423</v>
+      <c r="E23" t="s">
+        <v>491</v>
       </c>
       <c r="F23">
         <v>100156</v>
       </c>
       <c r="G23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80152","opis": "Зрењанин","sortiranje": 22,"brojRegistrovanihGlasaca":100156,"idUpravnogOkruga":"СРБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80152","opis": "Зрењанин","sortiranje": 22,"brojRegistrovanihGlasaca":100156,"idUpravnogOkruga":"СРБ","idPokrajine":"В"},</v>
       </c>
       <c r="H23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80152','Зрењанин',22,100156,'СРБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80152','Зрењанин',22,100156,'СРБ','В');</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -4007,19 +4003,19 @@
       <c r="D24" t="s">
         <v>396</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>423</v>
+      <c r="E24" t="s">
+        <v>491</v>
       </c>
       <c r="F24">
         <v>7992</v>
       </c>
       <c r="G24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80250","opis": "Нова Црња","sortiranje": 23,"brojRegistrovanihGlasaca":7992,"idUpravnogOkruga":"СРБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80250","opis": "Нова Црња","sortiranje": 23,"brojRegistrovanihGlasaca":7992,"idUpravnogOkruga":"СРБ","idPokrajine":"В"},</v>
       </c>
       <c r="H24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80250','Нова Црња',23,7992,'СРБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80250','Нова Црња',23,7992,'СРБ','В');</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -4036,19 +4032,19 @@
       <c r="D25" t="s">
         <v>396</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>423</v>
+      <c r="E25" t="s">
+        <v>491</v>
       </c>
       <c r="F25">
         <v>18708</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80268","opis": "Нови Бечеј","sortiranje": 24,"brojRegistrovanihGlasaca":18708,"idUpravnogOkruga":"СРБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80268","opis": "Нови Бечеј","sortiranje": 24,"brojRegistrovanihGlasaca":18708,"idUpravnogOkruga":"СРБ","idPokrajine":"В"},</v>
       </c>
       <c r="H25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80268','Нови Бечеј',24,18708,'СРБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80268','Нови Бечеј',24,18708,'СРБ','В');</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -4065,19 +4061,19 @@
       <c r="D26" t="s">
         <v>396</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>423</v>
+      <c r="E26" t="s">
+        <v>491</v>
       </c>
       <c r="F26">
         <v>10353</v>
       </c>
       <c r="G26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80373","opis": "Сечањ","sortiranje": 25,"brojRegistrovanihGlasaca":10353,"idUpravnogOkruga":"СРБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80373","opis": "Сечањ","sortiranje": 25,"brojRegistrovanihGlasaca":10353,"idUpravnogOkruga":"СРБ","idPokrajine":"В"},</v>
       </c>
       <c r="H26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80373','Сечањ',25,10353,'СРБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80373','Сечањ',25,10353,'СРБ','В');</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -4094,19 +4090,19 @@
       <c r="D27" t="s">
         <v>397</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>423</v>
+      <c r="E27" t="s">
+        <v>491</v>
       </c>
       <c r="F27">
         <v>14602</v>
       </c>
       <c r="G27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80012","opis": "Ада","sortiranje": 26,"brojRegistrovanihGlasaca":14602,"idUpravnogOkruga":"СВБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80012","opis": "Ада","sortiranje": 26,"brojRegistrovanihGlasaca":14602,"idUpravnogOkruga":"СВБ","idPokrajine":"В"},</v>
       </c>
       <c r="H27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80012','Ада',26,14602,'СВБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80012','Ада',26,14602,'СВБ','В');</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -4123,19 +4119,19 @@
       <c r="D28" t="s">
         <v>397</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>423</v>
+      <c r="E28" t="s">
+        <v>491</v>
       </c>
       <c r="F28">
         <v>21098</v>
       </c>
       <c r="G28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80195","opis": "Кањижа","sortiranje": 27,"brojRegistrovanihGlasaca":21098,"idUpravnogOkruga":"СВБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80195","opis": "Кањижа","sortiranje": 27,"brojRegistrovanihGlasaca":21098,"idUpravnogOkruga":"СВБ","idPokrajine":"В"},</v>
       </c>
       <c r="H28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80195','Кањижа',27,21098,'СВБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80195','Кањижа',27,21098,'СВБ','В');</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -4152,19 +4148,19 @@
       <c r="D29" t="s">
         <v>397</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>423</v>
+      <c r="E29" t="s">
+        <v>491</v>
       </c>
       <c r="F29">
         <v>47211</v>
       </c>
       <c r="G29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80209","opis": "Кикинда","sortiranje": 28,"brojRegistrovanihGlasaca":47211,"idUpravnogOkruga":"СВБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80209","opis": "Кикинда","sortiranje": 28,"brojRegistrovanihGlasaca":47211,"idUpravnogOkruga":"СВБ","idPokrajine":"В"},</v>
       </c>
       <c r="H29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80209','Кикинда',28,47211,'СВБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80209','Кикинда',28,47211,'СВБ','В');</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -4181,19 +4177,19 @@
       <c r="D30" t="s">
         <v>397</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>423</v>
+      <c r="E30" t="s">
+        <v>491</v>
       </c>
       <c r="F30">
         <v>8579</v>
       </c>
       <c r="G30" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80276","opis": "Нови Кнежевац","sortiranje": 29,"brojRegistrovanihGlasaca":8579,"idUpravnogOkruga":"СВБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80276","opis": "Нови Кнежевац","sortiranje": 29,"brojRegistrovanihGlasaca":8579,"idUpravnogOkruga":"СВБ","idPokrajine":"В"},</v>
       </c>
       <c r="H30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80276','Нови Кнежевац',29,8579,'СВБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80276','Нови Кнежевац',29,8579,'СВБ','В');</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -4210,19 +4206,19 @@
       <c r="D31" t="s">
         <v>397</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>423</v>
+      <c r="E31" t="s">
+        <v>491</v>
       </c>
       <c r="F31">
         <v>19690</v>
       </c>
       <c r="G31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80365","opis": "Сента","sortiranje": 30,"brojRegistrovanihGlasaca":19690,"idUpravnogOkruga":"СВБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80365","opis": "Сента","sortiranje": 30,"brojRegistrovanihGlasaca":19690,"idUpravnogOkruga":"СВБ","idPokrajine":"В"},</v>
       </c>
       <c r="H31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80365','Сента',30,19690,'СВБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80365','Сента',30,19690,'СВБ','В');</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -4239,19 +4235,19 @@
       <c r="D32" t="s">
         <v>397</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>423</v>
+      <c r="E32" t="s">
+        <v>491</v>
       </c>
       <c r="F32">
         <v>8871</v>
       </c>
       <c r="G32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80489","opis": "Чока","sortiranje": 31,"brojRegistrovanihGlasaca":8871,"idUpravnogOkruga":"СВБ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80489","opis": "Чока","sortiranje": 31,"brojRegistrovanihGlasaca":8871,"idUpravnogOkruga":"СВБ","idPokrajine":"В"},</v>
       </c>
       <c r="H32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80489','Чока',31,8871,'СВБ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80489','Чока',31,8871,'СВБ','В');</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -4268,19 +4264,19 @@
       <c r="D33" t="s">
         <v>398</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>423</v>
+      <c r="E33" t="s">
+        <v>491</v>
       </c>
       <c r="F33">
         <v>16980</v>
       </c>
       <c r="G33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80039","opis": "Алибунар","sortiranje": 32,"brojRegistrovanihGlasaca":16980,"idUpravnogOkruga":"ЈБН","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80039","opis": "Алибунар","sortiranje": 32,"brojRegistrovanihGlasaca":16980,"idUpravnogOkruga":"ЈБН","idPokrajine":"В"},</v>
       </c>
       <c r="H33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80039','Алибунар',32,16980,'ЈБН','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80039','Алибунар',32,16980,'ЈБН','В');</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -4297,19 +4293,19 @@
       <c r="D34" t="s">
         <v>398</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>423</v>
+      <c r="E34" t="s">
+        <v>491</v>
       </c>
       <c r="F34">
         <v>15632</v>
       </c>
       <c r="G34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80098","opis": "Бела Црква","sortiranje": 33,"brojRegistrovanihGlasaca":15632,"idUpravnogOkruga":"ЈБН","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80098","opis": "Бела Црква","sortiranje": 33,"brojRegistrovanihGlasaca":15632,"idUpravnogOkruga":"ЈБН","idPokrajine":"В"},</v>
       </c>
       <c r="H34" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80098','Бела Црква',33,15632,'ЈБН','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80098','Бела Црква',33,15632,'ЈБН','В');</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -4326,19 +4322,19 @@
       <c r="D35" t="s">
         <v>398</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>423</v>
+      <c r="E35" t="s">
+        <v>491</v>
       </c>
       <c r="F35">
         <v>44390</v>
       </c>
       <c r="G35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80128","opis": "Вршац","sortiranje": 34,"brojRegistrovanihGlasaca":44390,"idUpravnogOkruga":"ЈБН","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80128","opis": "Вршац","sortiranje": 34,"brojRegistrovanihGlasaca":44390,"idUpravnogOkruga":"ЈБН","idPokrajine":"В"},</v>
       </c>
       <c r="H35" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80128','Вршац',34,44390,'ЈБН','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80128','Вршац',34,44390,'ЈБН','В');</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -4355,19 +4351,19 @@
       <c r="D36" t="s">
         <v>398</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>423</v>
+      <c r="E36" t="s">
+        <v>491</v>
       </c>
       <c r="F36">
         <v>21089</v>
       </c>
       <c r="G36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80217","opis": "Ковачица","sortiranje": 35,"brojRegistrovanihGlasaca":21089,"idUpravnogOkruga":"ЈБН","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80217","opis": "Ковачица","sortiranje": 35,"brojRegistrovanihGlasaca":21089,"idUpravnogOkruga":"ЈБН","idPokrajine":"В"},</v>
       </c>
       <c r="H36" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80217','Ковачица',35,21089,'ЈБН','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80217','Ковачица',35,21089,'ЈБН','В');</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -4384,19 +4380,19 @@
       <c r="D37" t="s">
         <v>398</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>423</v>
+      <c r="E37" t="s">
+        <v>491</v>
       </c>
       <c r="F37">
         <v>27772</v>
       </c>
       <c r="G37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80225","opis": "Ковин","sortiranje": 36,"brojRegistrovanihGlasaca":27772,"idUpravnogOkruga":"ЈБН","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80225","opis": "Ковин","sortiranje": 36,"brojRegistrovanihGlasaca":27772,"idUpravnogOkruga":"ЈБН","idPokrajine":"В"},</v>
       </c>
       <c r="H37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80225','Ковин',36,27772,'ЈБН','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80225','Ковин',36,27772,'ЈБН','В');</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -4413,19 +4409,19 @@
       <c r="D38" t="s">
         <v>398</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>423</v>
+      <c r="E38" t="s">
+        <v>491</v>
       </c>
       <c r="F38">
         <v>8061</v>
       </c>
       <c r="G38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80292","opis": "Опово","sortiranje": 37,"brojRegistrovanihGlasaca":8061,"idUpravnogOkruga":"ЈБН","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80292","opis": "Опово","sortiranje": 37,"brojRegistrovanihGlasaca":8061,"idUpravnogOkruga":"ЈБН","idPokrajine":"В"},</v>
       </c>
       <c r="H38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80292','Опово',37,8061,'ЈБН','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80292','Опово',37,8061,'ЈБН','В');</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -4442,19 +4438,19 @@
       <c r="D39" t="s">
         <v>398</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>423</v>
+      <c r="E39" t="s">
+        <v>491</v>
       </c>
       <c r="F39">
         <v>106558</v>
       </c>
       <c r="G39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80314","opis": "Панчево","sortiranje": 38,"brojRegistrovanihGlasaca":106558,"idUpravnogOkruga":"ЈБН","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80314","opis": "Панчево","sortiranje": 38,"brojRegistrovanihGlasaca":106558,"idUpravnogOkruga":"ЈБН","idPokrajine":"В"},</v>
       </c>
       <c r="H39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80314','Панчево',38,106558,'ЈБН','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80314','Панчево',38,106558,'ЈБН','В');</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -4471,19 +4467,19 @@
       <c r="D40" t="s">
         <v>398</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>423</v>
+      <c r="E40" t="s">
+        <v>491</v>
       </c>
       <c r="F40">
         <v>8612</v>
       </c>
       <c r="G40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80349","opis": "Пландиште","sortiranje": 39,"brojRegistrovanihGlasaca":8612,"idUpravnogOkruga":"ЈБН","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80349","opis": "Пландиште","sortiranje": 39,"brojRegistrovanihGlasaca":8612,"idUpravnogOkruga":"ЈБН","idPokrajine":"В"},</v>
       </c>
       <c r="H40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80349','Пландиште',39,8612,'ЈБН','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80349','Пландиште',39,8612,'ЈБН','В');</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -4500,19 +4496,19 @@
       <c r="D41" t="s">
         <v>399</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>423</v>
+      <c r="E41" t="s">
+        <v>491</v>
       </c>
       <c r="F41">
         <v>24121</v>
       </c>
       <c r="G41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80047","opis": "Апатин","sortiranje": 40,"brojRegistrovanihGlasaca":24121,"idUpravnogOkruga":"ЗБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80047","opis": "Апатин","sortiranje": 40,"brojRegistrovanihGlasaca":24121,"idUpravnogOkruga":"ЗБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H41" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80047','Апатин',40,24121,'ЗБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80047','Апатин',40,24121,'ЗБЧ','В');</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -4529,19 +4525,19 @@
       <c r="D42" t="s">
         <v>399</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>423</v>
+      <c r="E42" t="s">
+        <v>491</v>
       </c>
       <c r="F42">
         <v>33931</v>
       </c>
       <c r="G42" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80233","opis": "Кула","sortiranje": 41,"brojRegistrovanihGlasaca":33931,"idUpravnogOkruga":"ЗБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80233","opis": "Кула","sortiranje": 41,"brojRegistrovanihGlasaca":33931,"idUpravnogOkruga":"ЗБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H42" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80233','Кула',41,33931,'ЗБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80233','Кула',41,33931,'ЗБЧ','В');</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -4558,19 +4554,19 @@
       <c r="D43" t="s">
         <v>399</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>423</v>
+      <c r="E43" t="s">
+        <v>491</v>
       </c>
       <c r="F43">
         <v>24127</v>
       </c>
       <c r="G43" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80306","opis": "Оџаци","sortiranje": 42,"brojRegistrovanihGlasaca":24127,"idUpravnogOkruga":"ЗБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80306","opis": "Оџаци","sortiranje": 42,"brojRegistrovanihGlasaca":24127,"idUpravnogOkruga":"ЗБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H43" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80306','Оџаци',42,24127,'ЗБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80306','Оџаци',42,24127,'ЗБЧ','В');</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -4587,19 +4583,19 @@
       <c r="D44" t="s">
         <v>399</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>423</v>
+      <c r="E44" t="s">
+        <v>491</v>
       </c>
       <c r="F44">
         <v>71505</v>
       </c>
       <c r="G44" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80381","opis": "Сомбор","sortiranje": 43,"brojRegistrovanihGlasaca":71505,"idUpravnogOkruga":"ЗБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80381","opis": "Сомбор","sortiranje": 43,"brojRegistrovanihGlasaca":71505,"idUpravnogOkruga":"ЗБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H44" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80381','Сомбор',43,71505,'ЗБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80381','Сомбор',43,71505,'ЗБЧ','В');</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -4616,19 +4612,19 @@
       <c r="D45" t="s">
         <v>400</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>423</v>
+      <c r="E45" t="s">
+        <v>491</v>
       </c>
       <c r="F45">
         <v>12149</v>
       </c>
       <c r="G45" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80055","opis": "Бач","sortiranje": 44,"brojRegistrovanihGlasaca":12149,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80055","opis": "Бач","sortiranje": 44,"brojRegistrovanihGlasaca":12149,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H45" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80055','Бач',44,12149,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80055','Бач',44,12149,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -4645,19 +4641,19 @@
       <c r="D46" t="s">
         <v>400</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>423</v>
+      <c r="E46" t="s">
+        <v>491</v>
       </c>
       <c r="F46">
         <v>45265</v>
       </c>
       <c r="G46" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80063","opis": "Бачка Паланка","sortiranje": 45,"brojRegistrovanihGlasaca":45265,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80063","opis": "Бачка Паланка","sortiranje": 45,"brojRegistrovanihGlasaca":45265,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H46" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80063','Бачка Паланка',45,45265,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80063','Бачка Паланка',45,45265,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -4674,19 +4670,19 @@
       <c r="D47" t="s">
         <v>400</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>423</v>
+      <c r="E47" t="s">
+        <v>491</v>
       </c>
       <c r="F47">
         <v>11735</v>
       </c>
       <c r="G47" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80080","opis": "Бачки Петровац","sortiranje": 46,"brojRegistrovanihGlasaca":11735,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80080","opis": "Бачки Петровац","sortiranje": 46,"brojRegistrovanihGlasaca":11735,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H47" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80080','Бачки Петровац',46,11735,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80080','Бачки Петровац',46,11735,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -4703,19 +4699,19 @@
       <c r="D48" t="s">
         <v>400</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>423</v>
+      <c r="E48" t="s">
+        <v>491</v>
       </c>
       <c r="F48">
         <v>13435</v>
       </c>
       <c r="G48" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80101","opis": "Беочин","sortiranje": 47,"brojRegistrovanihGlasaca":13435,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80101","opis": "Беочин","sortiranje": 47,"brojRegistrovanihGlasaca":13435,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H48" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80101','Беочин',47,13435,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80101','Беочин',47,13435,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -4732,19 +4728,19 @@
       <c r="D49" t="s">
         <v>400</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>423</v>
+      <c r="E49" t="s">
+        <v>491</v>
       </c>
       <c r="F49">
         <v>31679</v>
       </c>
       <c r="G49" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80110","opis": "Бечеј","sortiranje": 48,"brojRegistrovanihGlasaca":31679,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80110","opis": "Бечеј","sortiranje": 48,"brojRegistrovanihGlasaca":31679,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H49" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80110','Бечеј',48,31679,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80110','Бечеј',48,31679,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -4761,19 +4757,19 @@
       <c r="D50" t="s">
         <v>400</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>423</v>
+      <c r="E50" t="s">
+        <v>491</v>
       </c>
       <c r="F50">
         <v>21284</v>
       </c>
       <c r="G50" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80136","opis": "Жабаљ","sortiranje": 49,"brojRegistrovanihGlasaca":21284,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80136","opis": "Жабаљ","sortiranje": 49,"brojRegistrovanihGlasaca":21284,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H50" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80136','Жабаљ',49,21284,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80136','Жабаљ',49,21284,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -4790,19 +4786,19 @@
       <c r="D51" t="s">
         <v>400</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>423</v>
+      <c r="E51" t="s">
+        <v>491</v>
       </c>
       <c r="F51">
         <v>337233</v>
       </c>
       <c r="G51" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80284","opis": "Нови Сад","sortiranje": 50,"brojRegistrovanihGlasaca":337233,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80284","opis": "Нови Сад","sortiranje": 50,"brojRegistrovanihGlasaca":337233,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H51" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80284','Нови Сад',50,337233,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80284','Нови Сад',50,337233,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -4819,19 +4815,19 @@
       <c r="D52" t="s">
         <v>400</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>423</v>
+      <c r="E52" t="s">
+        <v>491</v>
       </c>
       <c r="F52">
         <v>13382</v>
       </c>
       <c r="G52" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80390","opis": "Србобран","sortiranje": 51,"brojRegistrovanihGlasaca":13382,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80390","opis": "Србобран","sortiranje": 51,"brojRegistrovanihGlasaca":13382,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H52" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80390','Србобран',51,13382,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80390','Србобран',51,13382,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -4848,19 +4844,19 @@
       <c r="D53" t="s">
         <v>400</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>423</v>
+      <c r="E53" t="s">
+        <v>491</v>
       </c>
       <c r="F53">
         <v>8076</v>
       </c>
       <c r="G53" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80411","opis": "Сремски Карловци","sortiranje": 52,"brojRegistrovanihGlasaca":8076,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80411","opis": "Сремски Карловци","sortiranje": 52,"brojRegistrovanihGlasaca":8076,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H53" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80411','Сремски Карловци',52,8076,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80411','Сремски Карловци',52,8076,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -4877,19 +4873,19 @@
       <c r="D54" t="s">
         <v>400</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>423</v>
+      <c r="E54" t="s">
+        <v>491</v>
       </c>
       <c r="F54">
         <v>24759</v>
       </c>
       <c r="G54" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80446","opis": "Темерин","sortiranje": 53,"brojRegistrovanihGlasaca":24759,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80446","opis": "Темерин","sortiranje": 53,"brojRegistrovanihGlasaca":24759,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H54" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80446','Темерин',53,24759,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80446','Темерин',53,24759,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -4906,19 +4902,19 @@
       <c r="D55" t="s">
         <v>400</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>423</v>
+      <c r="E55" t="s">
+        <v>491</v>
       </c>
       <c r="F55">
         <v>12714</v>
       </c>
       <c r="G55" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80454","opis": "Тител","sortiranje": 54,"brojRegistrovanihGlasaca":12714,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80454","opis": "Тител","sortiranje": 54,"brojRegistrovanihGlasaca":12714,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H55" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80454','Тител',54,12714,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80454','Тител',54,12714,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -4935,19 +4931,19 @@
       <c r="D56" t="s">
         <v>400</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>423</v>
+      <c r="E56" t="s">
+        <v>491</v>
       </c>
       <c r="F56">
         <v>33750</v>
       </c>
       <c r="G56" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80462","opis": "Врбас","sortiranje": 55,"brojRegistrovanihGlasaca":33750,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80462","opis": "Врбас","sortiranje": 55,"brojRegistrovanihGlasaca":33750,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80462','Врбас',55,33750,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80462','Врбас',55,33750,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -4964,19 +4960,19 @@
       <c r="D57" t="s">
         <v>400</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>423</v>
+      <c r="E57" t="s">
+        <v>491</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80519","opis": "Петроварадин","sortiranje": 56,"brojRegistrovanihGlasaca":0,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80519","opis": "Петроварадин","sortiranje": 56,"brojRegistrovanihGlasaca":0,"idUpravnogOkruga":"ЈБЧ","idPokrajine":"В"},</v>
       </c>
       <c r="H57" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80519','Петроварадин',56,0,'ЈБЧ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80519','Петроварадин',56,0,'ЈБЧ','В');</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -4993,19 +4989,19 @@
       <c r="D58" t="s">
         <v>401</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>423</v>
+      <c r="E58" t="s">
+        <v>491</v>
       </c>
       <c r="F58">
         <v>40540</v>
       </c>
       <c r="G58" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80179","opis": "Инђија","sortiranje": 57,"brojRegistrovanihGlasaca":40540,"idUpravnogOkruga":"СРМ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80179","opis": "Инђија","sortiranje": 57,"brojRegistrovanihGlasaca":40540,"idUpravnogOkruga":"СРМ","idPokrajine":"В"},</v>
       </c>
       <c r="H58" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80179','Инђија',57,40540,'СРМ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80179','Инђија',57,40540,'СРМ','В');</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -5022,19 +5018,19 @@
       <c r="D59" t="s">
         <v>401</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>423</v>
+      <c r="E59" t="s">
+        <v>491</v>
       </c>
       <c r="F59">
         <v>9052</v>
       </c>
       <c r="G59" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80187","opis": "Ириг","sortiranje": 58,"brojRegistrovanihGlasaca":9052,"idUpravnogOkruga":"СРМ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80187","opis": "Ириг","sortiranje": 58,"brojRegistrovanihGlasaca":9052,"idUpravnogOkruga":"СРМ","idPokrajine":"В"},</v>
       </c>
       <c r="H59" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80187','Ириг',58,9052,'СРМ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80187','Ириг',58,9052,'СРМ','В');</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -5051,19 +5047,19 @@
       <c r="D60" t="s">
         <v>401</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>423</v>
+      <c r="E60" t="s">
+        <v>491</v>
       </c>
       <c r="F60">
         <v>15594</v>
       </c>
       <c r="G60" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80322","opis": "Пећинци","sortiranje": 59,"brojRegistrovanihGlasaca":15594,"idUpravnogOkruga":"СРМ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80322","opis": "Пећинци","sortiranje": 59,"brojRegistrovanihGlasaca":15594,"idUpravnogOkruga":"СРМ","idPokrajine":"В"},</v>
       </c>
       <c r="H60" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80322','Пећинци',59,15594,'СРМ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80322','Пећинци',59,15594,'СРМ','В');</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -5080,19 +5076,19 @@
       <c r="D61" t="s">
         <v>401</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>423</v>
+      <c r="E61" t="s">
+        <v>491</v>
       </c>
       <c r="F61">
         <v>45692</v>
       </c>
       <c r="G61" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80357","opis": "Рума","sortiranje": 60,"brojRegistrovanihGlasaca":45692,"idUpravnogOkruga":"СРМ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80357","opis": "Рума","sortiranje": 60,"brojRegistrovanihGlasaca":45692,"idUpravnogOkruga":"СРМ","idPokrajine":"В"},</v>
       </c>
       <c r="H61" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80357','Рума',60,45692,'СРМ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80357','Рума',60,45692,'СРМ','В');</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -5109,19 +5105,19 @@
       <c r="D62" t="s">
         <v>401</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>423</v>
+      <c r="E62" t="s">
+        <v>491</v>
       </c>
       <c r="F62">
         <v>68761</v>
       </c>
       <c r="G62" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    {"idOpstine": "80403","opis": "Сремска Митровица","sortiranje": 61,"brojRegistrovanihGlasaca":68761,"idUpravnogOkruga":"СРМ","idPokrajine":"V"},</v>
+        <v xml:space="preserve">    {"idOpstine": "80403","opis": "Сремска Митровица","sortiranje": 61,"brojRegistrovanihGlasaca":68761,"idUpravnogOkruga":"СРМ","idPokrajine":"В"},</v>
       </c>
       <c r="H62" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80403','Сремска Митровица',61,68761,'СРМ','V');</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('80403','Сремска Митровица',61,68761,'СРМ','В');</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -5862,7 +5858,7 @@
         <v>179</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D90" t="s">
         <v>405</v>
@@ -5892,7 +5888,7 @@
         <v>181</v>
       </c>
       <c r="D91" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91">
@@ -5919,7 +5915,7 @@
         <v>183</v>
       </c>
       <c r="D92" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92">
@@ -5946,7 +5942,7 @@
         <v>185</v>
       </c>
       <c r="D93" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93">
@@ -5973,7 +5969,7 @@
         <v>187</v>
       </c>
       <c r="D94" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94">
@@ -6000,7 +5996,7 @@
         <v>189</v>
       </c>
       <c r="D95" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95">
@@ -6027,7 +6023,7 @@
         <v>191</v>
       </c>
       <c r="D96" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96">
@@ -6054,7 +6050,7 @@
         <v>193</v>
       </c>
       <c r="D97" t="s">
-        <v>406</v>
+        <v>422</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97">
@@ -6062,11 +6058,11 @@
       </c>
       <c r="G97" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">    {"idOpstine": "71277","opis": "Лапово","sortiranje": 96,"brojRegistrovanihGlasaca":6472,"idUpravnogOkruga":"ШУМ","idPokrajine":""},</v>
+        <v xml:space="preserve">    {"idOpstine": "71277","opis": "Лапово","sortiranje": 96,"brojRegistrovanihGlasaca":6472,"idUpravnogOkruga":"ШМД","idPokrajine":""},</v>
       </c>
       <c r="H97" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('71277','Лапово',96,6472,'ШУМ',null);</v>
+        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('71277','Лапово',96,6472,'ШМД',null);</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -6081,7 +6077,7 @@
         <v>195</v>
       </c>
       <c r="D98" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98">
@@ -6108,7 +6104,7 @@
         <v>198</v>
       </c>
       <c r="D99" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99">
@@ -6135,7 +6131,7 @@
         <v>200</v>
       </c>
       <c r="D100" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100">
@@ -6162,7 +6158,7 @@
         <v>202</v>
       </c>
       <c r="D101" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101">
@@ -6189,7 +6185,7 @@
         <v>204</v>
       </c>
       <c r="D102" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102">
@@ -6216,7 +6212,7 @@
         <v>206</v>
       </c>
       <c r="D103" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103">
@@ -6243,7 +6239,7 @@
         <v>208</v>
       </c>
       <c r="D104" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104">
@@ -6270,7 +6266,7 @@
         <v>210</v>
       </c>
       <c r="D105" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105">
@@ -6297,7 +6293,7 @@
         <v>212</v>
       </c>
       <c r="D106" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106">
@@ -6324,7 +6320,7 @@
         <v>214</v>
       </c>
       <c r="D107" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107">
@@ -6351,7 +6347,7 @@
         <v>216</v>
       </c>
       <c r="D108" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108">
@@ -6378,7 +6374,7 @@
         <v>218</v>
       </c>
       <c r="D109" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109">
@@ -6405,7 +6401,7 @@
         <v>220</v>
       </c>
       <c r="D110" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110">
@@ -6432,7 +6428,7 @@
         <v>223</v>
       </c>
       <c r="D111" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111">
@@ -6459,7 +6455,7 @@
         <v>225</v>
       </c>
       <c r="D112" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112">
@@ -6486,7 +6482,7 @@
         <v>227</v>
       </c>
       <c r="D113" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113">
@@ -6513,7 +6509,7 @@
         <v>229</v>
       </c>
       <c r="D114" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114">
@@ -6540,7 +6536,7 @@
         <v>231</v>
       </c>
       <c r="D115" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115">
@@ -6567,7 +6563,7 @@
         <v>233</v>
       </c>
       <c r="D116" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116">
@@ -6594,7 +6590,7 @@
         <v>235</v>
       </c>
       <c r="D117" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E117" s="2"/>
       <c r="F117">
@@ -6621,7 +6617,7 @@
         <v>237</v>
       </c>
       <c r="D118" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118">
@@ -6648,7 +6644,7 @@
         <v>239</v>
       </c>
       <c r="D119" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119">
@@ -6675,7 +6671,7 @@
         <v>242</v>
       </c>
       <c r="D120" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120">
@@ -6702,7 +6698,7 @@
         <v>241</v>
       </c>
       <c r="D121" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121">
@@ -6729,7 +6725,7 @@
         <v>244</v>
       </c>
       <c r="D122" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E122" s="2"/>
       <c r="F122">
@@ -6756,7 +6752,7 @@
         <v>246</v>
       </c>
       <c r="D123" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123">
@@ -6783,7 +6779,7 @@
         <v>248</v>
       </c>
       <c r="D124" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124">
@@ -6810,7 +6806,7 @@
         <v>250</v>
       </c>
       <c r="D125" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125">
@@ -6837,7 +6833,7 @@
         <v>252</v>
       </c>
       <c r="D126" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126">
@@ -6864,7 +6860,7 @@
         <v>254</v>
       </c>
       <c r="D127" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127">
@@ -6891,7 +6887,7 @@
         <v>256</v>
       </c>
       <c r="D128" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128">
@@ -6918,7 +6914,7 @@
         <v>258</v>
       </c>
       <c r="D129" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129">
@@ -6945,7 +6941,7 @@
         <v>260</v>
       </c>
       <c r="D130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130">
@@ -6972,7 +6968,7 @@
         <v>262</v>
       </c>
       <c r="D131" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131">
@@ -6999,7 +6995,7 @@
         <v>168</v>
       </c>
       <c r="D132" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E132"/>
       <c r="F132">
@@ -7026,7 +7022,7 @@
         <v>265</v>
       </c>
       <c r="D133" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133">
@@ -7053,7 +7049,7 @@
         <v>267</v>
       </c>
       <c r="D134" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134">
@@ -7080,7 +7076,7 @@
         <v>269</v>
       </c>
       <c r="D135" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135">
@@ -7107,7 +7103,7 @@
         <v>271</v>
       </c>
       <c r="D136" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136">
@@ -7134,7 +7130,7 @@
         <v>273</v>
       </c>
       <c r="D137" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137">
@@ -7161,7 +7157,7 @@
         <v>275</v>
       </c>
       <c r="D138" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138">
@@ -7188,7 +7184,7 @@
         <v>277</v>
       </c>
       <c r="D139" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139">
@@ -7215,7 +7211,7 @@
         <v>279</v>
       </c>
       <c r="D140" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140">
@@ -7242,7 +7238,7 @@
         <v>281</v>
       </c>
       <c r="D141" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E141" s="2"/>
       <c r="F141">
@@ -7269,7 +7265,7 @@
         <v>283</v>
       </c>
       <c r="D142" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E142" s="2"/>
       <c r="F142">
@@ -7296,7 +7292,7 @@
         <v>285</v>
       </c>
       <c r="D143" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E143" s="2"/>
       <c r="F143">
@@ -7323,7 +7319,7 @@
         <v>287</v>
       </c>
       <c r="D144" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E144" s="2"/>
       <c r="F144">
@@ -7350,7 +7346,7 @@
         <v>289</v>
       </c>
       <c r="D145" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E145" s="2"/>
       <c r="F145">
@@ -7377,7 +7373,7 @@
         <v>291</v>
       </c>
       <c r="D146" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E146" s="2"/>
       <c r="F146">
@@ -7404,7 +7400,7 @@
         <v>293</v>
       </c>
       <c r="D147" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E147" s="2"/>
       <c r="F147">
@@ -7431,7 +7427,7 @@
         <v>295</v>
       </c>
       <c r="D148" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E148" s="2"/>
       <c r="F148">
@@ -7458,7 +7454,7 @@
         <v>297</v>
       </c>
       <c r="D149" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E149" s="2"/>
       <c r="F149">
@@ -7485,7 +7481,7 @@
         <v>299</v>
       </c>
       <c r="D150" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E150" s="2"/>
       <c r="F150">
@@ -7512,7 +7508,7 @@
         <v>301</v>
       </c>
       <c r="D151" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E151" s="2"/>
       <c r="F151">
@@ -7539,7 +7535,7 @@
         <v>303</v>
       </c>
       <c r="D152" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E152" s="2"/>
       <c r="F152">
@@ -7566,7 +7562,7 @@
         <v>305</v>
       </c>
       <c r="D153" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E153" s="2"/>
       <c r="F153">
@@ -7593,7 +7589,7 @@
         <v>307</v>
       </c>
       <c r="D154" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E154" s="2"/>
       <c r="F154">
@@ -7620,7 +7616,7 @@
         <v>309</v>
       </c>
       <c r="D155" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E155" s="2"/>
       <c r="F155">
@@ -7647,7 +7643,7 @@
         <v>311</v>
       </c>
       <c r="D156" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E156" s="2"/>
       <c r="F156">
@@ -7674,7 +7670,7 @@
         <v>313</v>
       </c>
       <c r="D157" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E157" s="2"/>
       <c r="F157">
@@ -7701,7 +7697,7 @@
         <v>316</v>
       </c>
       <c r="D158" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E158" s="2"/>
       <c r="F158">
@@ -7728,7 +7724,7 @@
         <v>318</v>
       </c>
       <c r="D159" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E159" s="2"/>
       <c r="F159">
@@ -7755,7 +7751,7 @@
         <v>14</v>
       </c>
       <c r="D160" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E160" s="2"/>
       <c r="F160">
@@ -7782,7 +7778,7 @@
         <v>196</v>
       </c>
       <c r="D161" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E161" s="2"/>
       <c r="F161">
@@ -7809,7 +7805,7 @@
         <v>322</v>
       </c>
       <c r="D162" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E162" s="2"/>
       <c r="F162">
@@ -7836,7 +7832,7 @@
         <v>324</v>
       </c>
       <c r="D163" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E163" s="2"/>
       <c r="F163">
@@ -7863,7 +7859,7 @@
         <v>326</v>
       </c>
       <c r="D164" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E164" s="2"/>
       <c r="F164">
@@ -7890,7 +7886,7 @@
         <v>328</v>
       </c>
       <c r="D165" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E165" s="2"/>
       <c r="F165">
@@ -7917,7 +7913,7 @@
         <v>330</v>
       </c>
       <c r="D166" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E166" s="2"/>
       <c r="F166">
@@ -7944,7 +7940,7 @@
         <v>332</v>
       </c>
       <c r="D167" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E167" s="2"/>
       <c r="F167">
@@ -7971,7 +7967,7 @@
         <v>334</v>
       </c>
       <c r="D168" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E168" s="2"/>
       <c r="F168">
@@ -7998,7 +7994,7 @@
         <v>221</v>
       </c>
       <c r="D169" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E169" s="2"/>
       <c r="F169">
@@ -8025,7 +8021,7 @@
         <v>337</v>
       </c>
       <c r="D170" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E170" s="2"/>
       <c r="F170">
@@ -8052,7 +8048,7 @@
         <v>129</v>
       </c>
       <c r="D171" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E171" s="2"/>
       <c r="F171">
@@ -8079,7 +8075,7 @@
         <v>340</v>
       </c>
       <c r="D172" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E172" s="2"/>
       <c r="F172">
@@ -8106,7 +8102,7 @@
         <v>342</v>
       </c>
       <c r="D173" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E173" s="2"/>
       <c r="F173">
@@ -8133,7 +8129,7 @@
         <v>344</v>
       </c>
       <c r="D174" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E174" s="2"/>
       <c r="F174">
@@ -8160,7 +8156,7 @@
         <v>314</v>
       </c>
       <c r="D175" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E175" s="2"/>
       <c r="F175">
@@ -8187,7 +8183,7 @@
         <v>347</v>
       </c>
       <c r="D176" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E176" s="2"/>
       <c r="F176">
@@ -8214,7 +8210,7 @@
         <v>349</v>
       </c>
       <c r="D177" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E177" s="2"/>
       <c r="F177">
@@ -8241,7 +8237,7 @@
         <v>351</v>
       </c>
       <c r="D178" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E178" s="2"/>
       <c r="F178">
@@ -8268,7 +8264,7 @@
         <v>353</v>
       </c>
       <c r="D179" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E179" s="2"/>
       <c r="F179">
@@ -8295,7 +8291,7 @@
         <v>355</v>
       </c>
       <c r="D180" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E180" s="2"/>
       <c r="F180">
@@ -8322,7 +8318,7 @@
         <v>357</v>
       </c>
       <c r="D181" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E181" s="2"/>
       <c r="F181">
@@ -8349,7 +8345,7 @@
         <v>359</v>
       </c>
       <c r="D182" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E182" s="2"/>
       <c r="F182">
@@ -8376,7 +8372,7 @@
         <v>361</v>
       </c>
       <c r="D183" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E183" s="2"/>
       <c r="F183">
@@ -8403,7 +8399,7 @@
         <v>363</v>
       </c>
       <c r="D184" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E184" s="2"/>
       <c r="F184">
@@ -8430,7 +8426,7 @@
         <v>365</v>
       </c>
       <c r="D185" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E185" s="2"/>
       <c r="F185">
@@ -8457,7 +8453,7 @@
         <v>367</v>
       </c>
       <c r="D186" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E186" s="2"/>
       <c r="F186">
@@ -8484,7 +8480,7 @@
         <v>369</v>
       </c>
       <c r="D187" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E187" s="2"/>
       <c r="F187">
@@ -8511,7 +8507,7 @@
         <v>371</v>
       </c>
       <c r="D188" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E188" s="2"/>
       <c r="F188">
@@ -8538,7 +8534,7 @@
         <v>373</v>
       </c>
       <c r="D189" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E189" s="2"/>
       <c r="F189">
@@ -8565,7 +8561,7 @@
         <v>375</v>
       </c>
       <c r="D190" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E190" s="2"/>
       <c r="F190">
@@ -8592,7 +8588,7 @@
         <v>377</v>
       </c>
       <c r="D191" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E191" s="2"/>
       <c r="F191">
@@ -8619,7 +8615,7 @@
         <v>379</v>
       </c>
       <c r="D192" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E192" s="2"/>
       <c r="F192">
@@ -8646,7 +8642,7 @@
         <v>381</v>
       </c>
       <c r="D193" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E193" s="2"/>
       <c r="F193">
@@ -8673,7 +8669,7 @@
         <v>383</v>
       </c>
       <c r="D194" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E194" s="2"/>
       <c r="F194">
@@ -8700,7 +8696,7 @@
         <v>385</v>
       </c>
       <c r="D195" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E195" s="2"/>
       <c r="F195">
@@ -8727,7 +8723,7 @@
         <v>387</v>
       </c>
       <c r="D196" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E196" s="2"/>
       <c r="F196">
@@ -8754,7 +8750,7 @@
         <v>389</v>
       </c>
       <c r="D197" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E197" s="2"/>
       <c r="F197">
@@ -8781,7 +8777,7 @@
         <v>391</v>
       </c>
       <c r="D198" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E198" s="2"/>
       <c r="F198">
@@ -8808,7 +8804,7 @@
         <v>393</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E199" s="8"/>
       <c r="F199" s="6">
@@ -8832,10 +8828,6 @@
         <f>SUM(F2:F199)</f>
         <v>6488368</v>
       </c>
-      <c r="H200" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>insert into NIOpstina(IDNIOpstina, Opis, Sortiranje, BrojRegistrovanihGlasaca, IDNIUPravniOkrug, IDNIPokrajina) values ('','',,6488368,'',null);</v>
-      </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B201"/>

</xml_diff>